<commit_message>
Cập nhật kế hoạch bổ sung thông tin chi tiết vào dự án
</commit_message>
<xml_diff>
--- a/nop_bao_cao/xe2go_gantt_kehoachvietmanguon.xlsx
+++ b/nop_bao_cao/xe2go_gantt_kehoachvietmanguon.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe0b74459fd8554e/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xe2go\nop_bao_cao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC10480F199D7D4A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F11BFA-2FBF-446A-ABF9-B130FCABB90F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D3FECD-AFF9-4A3D-B965-64BE62E02632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch chung" sheetId="1" r:id="rId1"/>
+    <sheet name="Cập nhật mã nguồn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
   <si>
     <t>Tên công việc</t>
   </si>
@@ -109,13 +110,276 @@
   </si>
   <si>
     <t>Hướng dẫn Quý công ty về cách quản trị và cập nhật nội dung website.</t>
+  </si>
+  <si>
+    <t>ngày bắt đầu</t>
+  </si>
+  <si>
+    <t>ngày kết thúc</t>
+  </si>
+  <si>
+    <t>số giờ thực hiện</t>
+  </si>
+  <si>
+    <t>Chuẩn bị dữ liệu và thiết lập công cụ</t>
+  </si>
+  <si>
+    <t>Thu thập hình ảnh từ Zalo, tải về và phân loại thành các thư mục.</t>
+  </si>
+  <si>
+    <t>Sử dụng công cụ AI Photo Sorter để tự động phân loại hình ảnh.</t>
+  </si>
+  <si>
+    <t>Kiểm tra giải pháp lập trình hướng đối tượng đã xây dựng cho gallery (class FolderGallery và Fancybox) để đảm bảo sẵn sàng áp dụng.</t>
+  </si>
+  <si>
+    <t>Bắt đầu triển khai gallery</t>
+  </si>
+  <si>
+    <t>Phát triển giao diện trang chủ.</t>
+  </si>
+  <si>
+    <t>Tinh chỉnh và thử nghiệm toàn bộ hệ thống</t>
+  </si>
+  <si>
+    <t>Hoàn thiện và bàn giao bản demo.</t>
+  </si>
+  <si>
+    <t>Đánh giá và bàn giao chính thức</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tổng kết và bàn giao sản phẩm chính thức cho khách hàng.</t>
+  </si>
+  <si>
+    <t>Người thực hiện</t>
+  </si>
+  <si>
+    <t>Sok Kim Thanh
+Lê Duy Anh Tú</t>
+  </si>
+  <si>
+    <t>Mức ưu tiên công việc</t>
+  </si>
+  <si>
+    <t>Viết logic gallery và tích hợp Fancybox</t>
+  </si>
+  <si>
+    <t>Cấu hình Fancybox cho gallery, kiểm tra giao diện trên desktop và mobile. Kiểm tra Fancybox hoạt động đúng.</t>
+  </si>
+  <si>
+    <t>Hoàn chỉnh các phần liên quan đến slider trên menu và hình bảo hiểm cho trang chủ. Tinh chỉnh giao diện trang chủ</t>
+  </si>
+  <si>
+    <t>Soạn bản nháp kế hoạch công việc và phân chia nhiệm vụ cho đồng đội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gửi báo cáo tiến độ cho khách hàng: Báo cáo tiến độ qua email và nhận phản hồi từ khách hàng. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viết hướng dẫn sử dụng cho khách hàng: Soạn hướng dẫn quản trị website, cách sử dụng Fancybox, và cập nhật nội dung. </t>
+  </si>
+  <si>
+    <t>Chuẩn bị bản demo hoàn chỉnh: Tạo tệp nén toàn bộ dự án, bao gồm gallery và giao diện trang chủ.</t>
+  </si>
+  <si>
+    <t>Kiểm tra lần cuối cùng và bàn giao chính thức: Đánh giá toàn bộ hệ thống cùng đồng đội.</t>
+  </si>
+  <si>
+    <t>Xử lý các thay đổi nhỏ nếu có: Kiểm tra lần cuối các chức năng, đảm bảo không có lỗi.</t>
+  </si>
+  <si>
+    <t>Vấn đề và cải thiện</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vấn đề: Thu thập hình ảnh từ Zalo và phân loại có thể mất thời gian không cần thiết nếu hình ảnh không sẵn sàng hoặc chưa được khách hàng duyệt.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cải thiện:
+Gửi yêu cầu qua email/Zalo để khách hàng gửi hình ảnh đã được duyệt sớm nhất, tránh tình trạng thiếu hoặc sai hình.
+Nếu hình chưa sẵn sàng, tập trung vào xây dựng mã xử lý gallery trước để tiết kiệm thời gian.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vấn đề: Chỉnh sửa giao diện và tích hợp Fancybox trước khi gallery hoàn thiện có thể khiến việc kiểm tra toàn hệ thống phức tạp hơn.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cải thiện:
+Hoàn thành toàn bộ logic lập trình gallery trước, sau đó tích hợp Fancybox và tinh chỉnh giao diện song song với trang chủ.
+Phân chia nhiệm vụ rõ ràng: Một người xử lý mã gallery, một người tinh chỉnh giao diện.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vấn đề: Kiểm thử vào ngày 4 có thể không đủ thời gian để sửa lỗi nếu phát hiện vấn đề nghiêm trọng.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cải thiện:
+Tiến hành kiểm thử cơ bản ngay sau khi hoàn thành từng phần (gallery và trang chủ).
+Dành một phần của ngày 3 để bắt đầu kiểm thử sớm.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vấn đề: Để bàn giao chính thức vào ngày cuối cùng (hạn chót) có thể gây áp lực nếu phát hiện lỗi sát giờ.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cải thiện:
+Đặt mục tiêu hoàn thành bản demo và báo cáo tổng kết vào ngày 29/12.
+Ngày 30/12 chỉ dành cho việc kiểm tra lần cuối và xử lý phản hồi nhỏ, giảm thiểu rủi ro.</t>
+    </r>
+  </si>
+  <si>
+    <t>Viết mã PHP OOP hoàn thiện gallery và kiểm tra việc hiển thị danh sách hình ảnh trang chủ</t>
+  </si>
+  <si>
+    <t>Chuẩn bị thư mục hình ảnh và chỉnh sửa trang danh sách sản phẩm</t>
+  </si>
+  <si>
+    <t>Chuẩn bị thư mục hình ảnh và chỉnh sửa trang chủ</t>
+  </si>
+  <si>
+    <t>Thiết lập giải pháp lập trình hướng đối tượng cho gallery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xử lý phản hồi của khách hàng (nếu có): Thực hiện các chỉnh sửa cuối cùng dựa trên phản hồi của khách hàng.  </t>
+  </si>
+  <si>
+    <t>Kiểm thử toàn bộ hệ thống trên nhiều thiết bị và trình duyệt: Kiểm tra giao diện và chức năng trên nhiều trình duyệt và thiết bị.</t>
+  </si>
+  <si>
+    <t>Tối ưu hóa mã nguồn(CSS/JS gọn nhẹ, lazy loading): gộp và nén CSS/JS, kiểm tra lazy loading cho gallery.</t>
+  </si>
+  <si>
+    <t>Viết mã PHP OOP hoàn thiện gallery và kiểm tra việc hiển thị danh sách hình ảnh trang danh mục sản phẩm</t>
+  </si>
+  <si>
+    <t>Hiển thị các mục bổ sung trên trang chủ:
+Thêm các hình ảnh như cơ sở pháp lý, bảo hiểm.
+Tích hợp liên kết bảo hiểm vào footer.</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa kích thước hợp lý cho menu, logo, và các thành phần khác theo thiết kế trên màn hình laptop 1366px</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Cập nhật trạng thái công việc vào cuối ngày cho khách hàng và đồng đội.</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email yêu cầu khách hàng cung cấp hình ảnh đã duyệt.</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Cập nhật báo cáo tiến độ.</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email cho khách hàng kèm bản demo và các tài liệu liên quan.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +410,133 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -163,11 +544,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -177,29 +591,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -269,6 +708,24 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF222222"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1304,15 +1761,152 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5611005</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1552792</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{237C1CEF-513C-44DD-AE9A-0D9BB00A4C79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6896100" y="6362700"/>
+          <a:ext cx="5591955" cy="1552792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>20170</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>21851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3182911</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1860433</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE492FB4-DE9D-4EE2-8394-A99BC8E69D5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6900582" y="7574616"/>
+          <a:ext cx="3162741" cy="1838582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21852</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>20170</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3613278</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1220488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE52A18-9B62-4D4F-A217-DC2B434FC3B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6902264" y="9455523"/>
+          <a:ext cx="3591426" cy="1200318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{703F07F9-7C4F-48CD-A7BA-7563727F4EE5}" name="Table1" displayName="Table1" ref="B4:G17" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{703F07F9-7C4F-48CD-A7BA-7563727F4EE5}" name="Table1" displayName="Table1" ref="B4:G17" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B4:G17" xr:uid="{703F07F9-7C4F-48CD-A7BA-7563727F4EE5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{42F2E47B-6096-43D8-B54E-034E8A83E75A}" name="Giai đoạn" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{42F2E47B-6096-43D8-B54E-034E8A83E75A}" name="Giai đoạn" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{8CD5CADC-5038-438B-B278-ECD348378C3E}" name="Tên công việc"/>
-    <tableColumn id="3" xr3:uid="{AC4AD0EA-D833-4072-A86E-CCF0D3165D08}" name="Thành viên thực hiện" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8E9BCE39-129D-4C8E-96E2-1296C1222DB7}" name="Ngày bắt đầu" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{0452BE5B-DB52-44F6-89DC-E21AE61F6C8C}" name="Ngày kết thúc" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{AC4AD0EA-D833-4072-A86E-CCF0D3165D08}" name="Thành viên thực hiện" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{8E9BCE39-129D-4C8E-96E2-1296C1222DB7}" name="Ngày bắt đầu" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{0452BE5B-DB52-44F6-89DC-E21AE61F6C8C}" name="Ngày kết thúc" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{37D6A49B-E662-4F07-8FC3-55DDBFF9C668}" name="Số giờ làm việc một ngày"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1584,7 +2178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1896,4 +2490,674 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC3744B-6692-456B-A13C-CDD2B8AE7919}">
+  <dimension ref="C5:J37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="36.125" customWidth="1"/>
+    <col min="5" max="5" width="73.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="10"/>
+      <c r="E7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I7" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D8" s="10"/>
+      <c r="E8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="10"/>
+      <c r="E9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D10" s="10"/>
+      <c r="E10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D11" s="10"/>
+      <c r="E11" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I11" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D12" s="10"/>
+      <c r="E12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I12" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D13" s="10"/>
+      <c r="E13" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I13" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D14" s="10"/>
+      <c r="E14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3">
+        <v>45651</v>
+      </c>
+      <c r="I14" s="3">
+        <v>45652</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3">
+        <v>45652</v>
+      </c>
+      <c r="I15" s="3">
+        <v>45653</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D16" s="10"/>
+      <c r="E16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="3">
+        <v>45652</v>
+      </c>
+      <c r="I16" s="3">
+        <v>45653</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D17" s="10"/>
+      <c r="E17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3">
+        <v>45652</v>
+      </c>
+      <c r="I17" s="3">
+        <v>45653</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D18" s="10"/>
+      <c r="E18" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3">
+        <v>45652</v>
+      </c>
+      <c r="I18" s="3">
+        <v>45653</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I19" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D20" s="10"/>
+      <c r="E20" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I20" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D21" s="10"/>
+      <c r="E21" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I21" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D22" s="10"/>
+      <c r="E22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I22" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="10"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="8"/>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I23" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="10"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="8"/>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I24" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="10"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="8"/>
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I25" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D26" s="10"/>
+      <c r="E26" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="3">
+        <v>45653</v>
+      </c>
+      <c r="I26" s="3">
+        <v>45654</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="3">
+        <v>45654</v>
+      </c>
+      <c r="I27" s="3">
+        <v>45655</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D28" s="10"/>
+      <c r="E28" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="3">
+        <v>45654</v>
+      </c>
+      <c r="I28" s="3">
+        <v>45655</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D29" s="10"/>
+      <c r="E29" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="3">
+        <v>45654</v>
+      </c>
+      <c r="I29" s="3">
+        <v>45655</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D30" s="10"/>
+      <c r="E30" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="3">
+        <v>45654</v>
+      </c>
+      <c r="I30" s="3">
+        <v>45655</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="3">
+        <v>45655</v>
+      </c>
+      <c r="I31" s="3">
+        <v>45656</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D32" s="10"/>
+      <c r="E32" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="3">
+        <v>45655</v>
+      </c>
+      <c r="I32" s="3">
+        <v>45656</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D33" s="10"/>
+      <c r="E33" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="3">
+        <v>45655</v>
+      </c>
+      <c r="I33" s="3">
+        <v>45656</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="3">
+        <v>45656</v>
+      </c>
+      <c r="I34" s="3">
+        <v>45657</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D35" s="10"/>
+      <c r="E35" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="18"/>
+      <c r="G35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="3">
+        <v>45656</v>
+      </c>
+      <c r="I35" s="3">
+        <v>45657</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D36" s="10"/>
+      <c r="E36" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="27"/>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="3">
+        <v>45656</v>
+      </c>
+      <c r="I36" s="3">
+        <v>45657</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D37" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D15:D26"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="D6:D14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật tiến độ công việc đợt 2: soạn cấu trúc hiển thị và ghép nối dữ liệu
</commit_message>
<xml_diff>
--- a/nop_bao_cao/xe2go_gantt_kehoachvietmanguon.xlsx
+++ b/nop_bao_cao/xe2go_gantt_kehoachvietmanguon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xe2go\nop_bao_cao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D3FECD-AFF9-4A3D-B965-64BE62E02632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2DB40A-F8EE-43AB-93E0-9E5C11D171B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
   <si>
     <t>Tên công việc</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email cho khách hàng kèm bản demo và các tài liệu liên quan.</t>
+  </si>
+  <si>
+    <t>% hoàn thành</t>
   </si>
 </sst>
 </file>
@@ -581,25 +584,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -630,6 +627,39 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2190,14 +2220,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -2494,24 +2524,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC3744B-6692-456B-A13C-CDD2B8AE7919}">
-  <dimension ref="C5:J37"/>
+  <dimension ref="C5:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="36.125" customWidth="1"/>
     <col min="5" max="5" width="73.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2521,633 +2552,681 @@
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" t="s">
+      <c r="F6" s="29"/>
+      <c r="G6" s="11"/>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>45651</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>45652</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="10"/>
-      <c r="E7" s="12" t="s">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D7" s="28"/>
+      <c r="E7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" t="s">
+      <c r="F7" s="29"/>
+      <c r="G7" s="7"/>
+      <c r="H7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>45651</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>45652</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D8" s="10"/>
-      <c r="E8" s="9" t="s">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D8" s="28"/>
+      <c r="E8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" t="s">
+      <c r="F8" s="30">
+        <v>100</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>45651</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>45652</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D9" s="10"/>
-      <c r="E9" s="12" t="s">
+    <row r="9" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="28"/>
+      <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" t="s">
+      <c r="F9" s="29"/>
+      <c r="G9" s="7"/>
+      <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>45651</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>45652</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D10" s="10"/>
-      <c r="E10" s="9" t="s">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D10" s="28"/>
+      <c r="E10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" t="s">
+      <c r="F10" s="30">
+        <v>100</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>45651</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>45652</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D11" s="10"/>
-      <c r="E11" s="26" t="s">
+    <row r="11" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D11" s="28"/>
+      <c r="E11" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" t="s">
+      <c r="F11" s="31">
+        <v>100</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>45651</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>45652</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="10"/>
-      <c r="E12" s="9" t="s">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="28"/>
+      <c r="E12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" t="s">
+      <c r="F12" s="30">
+        <v>100</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>45651</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>45652</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D13" s="10"/>
-      <c r="E13" s="12" t="s">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D13" s="28"/>
+      <c r="E13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" t="s">
+      <c r="F13" s="30">
+        <v>100</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>45651</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>45652</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D14" s="10"/>
-      <c r="E14" s="12" t="s">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="28"/>
+      <c r="E14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="7"/>
+      <c r="H14" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>45651</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>45652</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" t="s">
+      <c r="F15" s="31">
+        <v>100</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>45652</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>45653</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D16" s="10"/>
-      <c r="E16" s="12" t="s">
+    <row r="16" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D16" s="28"/>
+      <c r="E16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" t="s">
+      <c r="F16" s="31">
+        <v>100</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>45652</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>45653</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D17" s="10"/>
-      <c r="E17" s="12" t="s">
+    <row r="17" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D17" s="28"/>
+      <c r="E17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="7"/>
+      <c r="H17" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>45652</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>45653</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D18" s="10"/>
-      <c r="E18" s="26" t="s">
+    <row r="18" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D18" s="28"/>
+      <c r="E18" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" t="s">
+      <c r="F18" s="33"/>
+      <c r="G18" s="17"/>
+      <c r="H18" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>45652</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>45653</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="12" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" t="s">
+      <c r="F19" s="32"/>
+      <c r="G19" s="7"/>
+      <c r="H19" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>45653</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>45654</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D20" s="10"/>
-      <c r="E20" s="12" t="s">
+    <row r="20" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D20" s="28"/>
+      <c r="E20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" t="s">
+      <c r="F20" s="32"/>
+      <c r="G20" s="7"/>
+      <c r="H20" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>45653</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>45654</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D21" s="10"/>
-      <c r="E21" s="25" t="s">
+    <row r="21" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D21" s="28"/>
+      <c r="E21" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" t="s">
+      <c r="F21" s="34"/>
+      <c r="G21" s="22"/>
+      <c r="H21" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>45653</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>45654</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D22" s="10"/>
-      <c r="E22" s="12" t="s">
+    <row r="22" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D22" s="28"/>
+      <c r="E22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="7"/>
+      <c r="H22" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>45653</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>45654</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="3:10" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="10"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="8"/>
-      <c r="G23" t="s">
+    <row r="23" spans="3:11" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="28"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="7"/>
+      <c r="H23" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>45653</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>45654</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="3:10" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="10"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="8"/>
-      <c r="G24" t="s">
+    <row r="24" spans="3:11" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="28"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="7"/>
+      <c r="H24" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>45653</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>45654</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="3:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="10"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="8"/>
-      <c r="G25" t="s">
+    <row r="25" spans="3:11" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="28"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="7"/>
+      <c r="H25" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <v>45653</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <v>45654</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D26" s="10"/>
-      <c r="E26" s="26" t="s">
+    <row r="26" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D26" s="28"/>
+      <c r="E26" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" t="s">
+      <c r="F26" s="33"/>
+      <c r="G26" s="18"/>
+      <c r="H26" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <v>45653</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>45654</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" t="s">
+      <c r="F27" s="32"/>
+      <c r="G27" s="13"/>
+      <c r="H27" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="3">
+      <c r="I27" s="3">
         <v>45654</v>
       </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
         <v>45655</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D28" s="10"/>
-      <c r="E28" s="12" t="s">
+    <row r="28" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D28" s="28"/>
+      <c r="E28" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="16"/>
-      <c r="G28" t="s">
+      <c r="F28" s="32"/>
+      <c r="G28" s="14"/>
+      <c r="H28" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="3">
+      <c r="I28" s="3">
         <v>45654</v>
       </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
         <v>45655</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D29" s="10"/>
-      <c r="E29" s="12" t="s">
+    <row r="29" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D29" s="28"/>
+      <c r="E29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="14"/>
+      <c r="H29" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="3">
+      <c r="I29" s="3">
         <v>45654</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <v>45655</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D30" s="10"/>
-      <c r="E30" s="26" t="s">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D30" s="28"/>
+      <c r="E30" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" t="s">
+      <c r="F30" s="33"/>
+      <c r="G30" s="12"/>
+      <c r="H30" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="3">
         <v>45654</v>
       </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
         <v>45655</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="12" t="s">
+      <c r="D31" s="28"/>
+      <c r="E31" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" t="s">
+      <c r="F31" s="32"/>
+      <c r="G31" s="14"/>
+      <c r="H31" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="3">
+      <c r="I31" s="3">
         <v>45655</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <v>45656</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D32" s="10"/>
-      <c r="E32" s="12" t="s">
+    <row r="32" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D32" s="28"/>
+      <c r="E32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="16"/>
-      <c r="G32" t="s">
+      <c r="F32" s="32"/>
+      <c r="G32" s="14"/>
+      <c r="H32" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="3">
         <v>45655</v>
       </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
         <v>45656</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D33" s="10"/>
-      <c r="E33" s="26" t="s">
+    <row r="33" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D33" s="28"/>
+      <c r="E33" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" t="s">
+      <c r="F33" s="33"/>
+      <c r="G33" s="19"/>
+      <c r="H33" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>45655</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>45656</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="7" t="s">
+      <c r="F34" s="32"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="3">
+      <c r="I34" s="3">
         <v>45656</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <v>45657</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D35" s="10"/>
-      <c r="E35" s="12" t="s">
+    <row r="35" spans="3:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="D35" s="28"/>
+      <c r="E35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="7" t="s">
+      <c r="F35" s="32"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H35" s="3">
+      <c r="I35" s="3">
         <v>45656</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <v>45657</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D36" s="10"/>
-      <c r="E36" s="28" t="s">
+    <row r="36" spans="3:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D36" s="28"/>
+      <c r="E36" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="G36" t="s">
+      <c r="F36" s="35"/>
+      <c r="G36" s="25"/>
+      <c r="H36" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="3">
+      <c r="I36" s="3">
         <v>45656</v>
       </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
         <v>45657</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D37" s="11"/>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D37" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
thêm thông tin trang gallery, đổi mới thư mục trang_gallery
</commit_message>
<xml_diff>
--- a/nop_bao_cao/xe2go_gantt_kehoachvietmanguon.xlsx
+++ b/nop_bao_cao/xe2go_gantt_kehoachvietmanguon.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xe2go\nop_bao_cao\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D3FECD-AFF9-4A3D-B965-64BE62E02632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch chung" sheetId="1" r:id="rId1"/>
     <sheet name="Cập nhật mã nguồn" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cập nhật mã nguồn'!$C$5:$J$36</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,6 +22,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,81 +33,90 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
   <si>
+    <t xml:space="preserve">Kế hoạch phát triển website tĩnh CÔNG TY TNHH QUỐC LONG BD </t>
+  </si>
+  <si>
+    <t>Giai đoạn</t>
+  </si>
+  <si>
     <t>Tên công việc</t>
   </si>
   <si>
-    <t>Giai đoạn</t>
+    <t>Thành viên thực hiện</t>
+  </si>
+  <si>
+    <t>Ngày bắt đầu</t>
+  </si>
+  <si>
+    <t>Ngày kết thúc</t>
+  </si>
+  <si>
+    <t>Số giờ làm việc một ngày</t>
+  </si>
+  <si>
+    <t>Đợt 1: Bàn giao khung sản phẩm không có nội dung (Xác nhận layout)</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện trang chủ</t>
+  </si>
+  <si>
+    <t>Sok Kim Thanh</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện trang gallery</t>
+  </si>
+  <si>
+    <t>Lê Duy Anh Tú</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện trang liên hệ;</t>
   </si>
   <si>
     <t>Đợt 2: Bàn giao sản phẩm có dữ liệu (Thêm dữ liệu)</t>
   </si>
   <si>
-    <t>Ngày bắt đầu</t>
-  </si>
-  <si>
-    <t>Ngày kết thúc</t>
+    <t>Thu thập và chuẩn bị nội dung từ hồ sơ năng lực của công ty xe2go;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chèn nội dung vào các trang tương ứng trên website; </t>
+  </si>
+  <si>
+    <t>đảm bảo định dạng và hiển thị nội dung chính xác, thẩm mỹ.</t>
   </si>
   <si>
     <t>Đợt 3: Bàn giao sản phẩm demo (Chạy thử trên local)</t>
   </si>
   <si>
-    <t>Đợt 1: Bàn giao khung sản phẩm không có nội dung (Xác nhận layout)</t>
-  </si>
-  <si>
-    <t>Thành viên thực hiện</t>
+    <t xml:space="preserve">Cài đặt và cấu hình môi trường phát triển trên máy tính cá nhân; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra các chức năng: điều hướng, gallery, biểu mẫu liên hệ; </t>
+  </si>
+  <si>
+    <t>Sửa lỗi và tối ưu hóa hiệu suất dựa trên kết quả kiểm tra.</t>
   </si>
   <si>
     <t>Đợt 4: Bàn giao sản phẩm chạy trên hosting</t>
   </si>
   <si>
-    <t>Thu thập và chuẩn bị nội dung từ hồ sơ năng lực của công ty xe2go;</t>
-  </si>
-  <si>
-    <t>Thiết kế giao diện trang gallery</t>
-  </si>
-  <si>
-    <t>Thiết kế giao diện trang liên hệ;</t>
-  </si>
-  <si>
-    <t>Thiết kế giao diện trang chủ</t>
-  </si>
-  <si>
-    <t>Sok Kim Thanh</t>
-  </si>
-  <si>
-    <t>Lê Duy Anh Tú</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cài đặt và cấu hình môi trường phát triển trên máy tính cá nhân; </t>
-  </si>
-  <si>
     <t xml:space="preserve">Lựa chọn và thiết lập hosting phù hợp với yêu cầu kỹ thuật của website; triển khai mã nguồn lên hosting; </t>
   </si>
   <si>
-    <t xml:space="preserve">Kế hoạch phát triển website tĩnh CÔNG TY TNHH QUỐC LONG BD </t>
-  </si>
-  <si>
-    <t>đảm bảo định dạng và hiển thị nội dung chính xác, thẩm mỹ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chèn nội dung vào các trang tương ứng trên website; </t>
-  </si>
-  <si>
-    <t>Số giờ làm việc một ngày</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra các chức năng: điều hướng, gallery, biểu mẫu liên hệ; </t>
-  </si>
-  <si>
-    <t>Sửa lỗi và tối ưu hóa hiệu suất dựa trên kết quả kiểm tra.</t>
-  </si>
-  <si>
     <t xml:space="preserve">kiểm tra lần cuối các chức năng trên môi trường trực tuyến; </t>
   </si>
   <si>
     <t>Hướng dẫn Quý công ty về cách quản trị và cập nhật nội dung website.</t>
   </si>
   <si>
+    <t>Vấn đề và cải thiện</t>
+  </si>
+  <si>
+    <t>Mức ưu tiên công việc</t>
+  </si>
+  <si>
+    <t>Người thực hiện</t>
+  </si>
+  <si>
     <t>ngày bắt đầu</t>
   </si>
   <si>
@@ -122,81 +127,14 @@
   </si>
   <si>
     <t>Chuẩn bị dữ liệu và thiết lập công cụ</t>
-  </si>
-  <si>
-    <t>Thu thập hình ảnh từ Zalo, tải về và phân loại thành các thư mục.</t>
-  </si>
-  <si>
-    <t>Sử dụng công cụ AI Photo Sorter để tự động phân loại hình ảnh.</t>
-  </si>
-  <si>
-    <t>Kiểm tra giải pháp lập trình hướng đối tượng đã xây dựng cho gallery (class FolderGallery và Fancybox) để đảm bảo sẵn sàng áp dụng.</t>
-  </si>
-  <si>
-    <t>Bắt đầu triển khai gallery</t>
-  </si>
-  <si>
-    <t>Phát triển giao diện trang chủ.</t>
-  </si>
-  <si>
-    <t>Tinh chỉnh và thử nghiệm toàn bộ hệ thống</t>
-  </si>
-  <si>
-    <t>Hoàn thiện và bàn giao bản demo.</t>
-  </si>
-  <si>
-    <t>Đánh giá và bàn giao chính thức</t>
-  </si>
-  <si>
-    <t>Gửi báo cáo tổng kết và bàn giao sản phẩm chính thức cho khách hàng.</t>
-  </si>
-  <si>
-    <t>Người thực hiện</t>
-  </si>
-  <si>
-    <t>Sok Kim Thanh
-Lê Duy Anh Tú</t>
-  </si>
-  <si>
-    <t>Mức ưu tiên công việc</t>
-  </si>
-  <si>
-    <t>Viết logic gallery và tích hợp Fancybox</t>
-  </si>
-  <si>
-    <t>Cấu hình Fancybox cho gallery, kiểm tra giao diện trên desktop và mobile. Kiểm tra Fancybox hoạt động đúng.</t>
-  </si>
-  <si>
-    <t>Hoàn chỉnh các phần liên quan đến slider trên menu và hình bảo hiểm cho trang chủ. Tinh chỉnh giao diện trang chủ</t>
-  </si>
-  <si>
-    <t>Soạn bản nháp kế hoạch công việc và phân chia nhiệm vụ cho đồng đội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gửi báo cáo tiến độ cho khách hàng: Báo cáo tiến độ qua email và nhận phản hồi từ khách hàng. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viết hướng dẫn sử dụng cho khách hàng: Soạn hướng dẫn quản trị website, cách sử dụng Fancybox, và cập nhật nội dung. </t>
-  </si>
-  <si>
-    <t>Chuẩn bị bản demo hoàn chỉnh: Tạo tệp nén toàn bộ dự án, bao gồm gallery và giao diện trang chủ.</t>
-  </si>
-  <si>
-    <t>Kiểm tra lần cuối cùng và bàn giao chính thức: Đánh giá toàn bộ hệ thống cùng đồng đội.</t>
-  </si>
-  <si>
-    <t>Xử lý các thay đổi nhỏ nếu có: Kiểm tra lần cuối các chức năng, đảm bảo không có lỗi.</t>
-  </si>
-  <si>
-    <t>Vấn đề và cải thiện</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Vấn đề: Thu thập hình ảnh từ Zalo và phân loại có thể mất thời gian không cần thiết nếu hình ảnh không sẵn sàng hoặc chưa được khách hàng duyệt.</t>
@@ -205,8 +143,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -216,8 +154,8 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Cải thiện:
@@ -226,12 +164,42 @@
     </r>
   </si>
   <si>
+    <t>Thu thập hình ảnh từ Zalo, tải về và phân loại thành các thư mục.</t>
+  </si>
+  <si>
+    <t>Sử dụng công cụ AI Photo Sorter để tự động phân loại hình ảnh.</t>
+  </si>
+  <si>
+    <t>Thiết lập giải pháp lập trình hướng đối tượng cho gallery</t>
+  </si>
+  <si>
+    <t>Kiểm tra giải pháp lập trình hướng đối tượng đã xây dựng cho gallery (class FolderGallery và Fancybox) để đảm bảo sẵn sàng áp dụng.</t>
+  </si>
+  <si>
+    <t>Soạn bản nháp kế hoạch công việc và phân chia nhiệm vụ cho đồng đội</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email yêu cầu khách hàng cung cấp hình ảnh đã duyệt.</t>
+  </si>
+  <si>
+    <t>Viết logic gallery và tích hợp Fancybox</t>
+  </si>
+  <si>
+    <t>Chuẩn bị thư mục hình ảnh và chỉnh sửa trang chủ</t>
+  </si>
+  <si>
+    <t>Chuẩn bị thư mục hình ảnh và chỉnh sửa trang danh sách sản phẩm</t>
+  </si>
+  <si>
+    <t>Bắt đầu triển khai gallery</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Vấn đề: Chỉnh sửa giao diện và tích hợp Fancybox trước khi gallery hoàn thiện có thể khiến việc kiểm tra toàn hệ thống phức tạp hơn.</t>
@@ -240,8 +208,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -251,8 +219,8 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Cải thiện:
@@ -261,12 +229,44 @@
     </r>
   </si>
   <si>
+    <t>Viết mã PHP OOP hoàn thiện gallery và kiểm tra việc hiển thị danh sách hình ảnh trang chủ</t>
+  </si>
+  <si>
+    <t>Cấu hình Fancybox cho gallery, kiểm tra giao diện trên desktop và mobile. Kiểm tra Fancybox hoạt động đúng.</t>
+  </si>
+  <si>
+    <t>Hoàn chỉnh các phần liên quan đến slider trên menu và hình bảo hiểm cho trang chủ. Tinh chỉnh giao diện trang chủ</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Cập nhật trạng thái công việc vào cuối ngày cho khách hàng và đồng đội.</t>
+  </si>
+  <si>
+    <t>Phát triển giao diện trang chủ.</t>
+  </si>
+  <si>
+    <t>Hiển thị các mục bổ sung trên trang chủ:
+Thêm các hình ảnh như cơ sở pháp lý, bảo hiểm.
+Tích hợp liên kết bảo hiểm vào footer.</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa kích thước hợp lý cho menu, logo, và các thành phần khác theo thiết kế trên màn hình laptop 1366px</t>
+  </si>
+  <si>
+    <t>Viết mã PHP OOP hoàn thiện gallery và kiểm tra việc hiển thị danh sách hình ảnh trang danh mục sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gửi báo cáo tiến độ cho khách hàng: Báo cáo tiến độ qua email và nhận phản hồi từ khách hàng. </t>
+  </si>
+  <si>
+    <t>Tinh chỉnh và thử nghiệm toàn bộ hệ thống</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Vấn đề: Kiểm thử vào ngày 4 có thể không đủ thời gian để sửa lỗi nếu phát hiện vấn đề nghiêm trọng.</t>
@@ -275,8 +275,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -286,8 +286,8 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Cải thiện:
@@ -296,12 +296,39 @@
     </r>
   </si>
   <si>
+    <t>Tối ưu hóa mã nguồn(CSS/JS gọn nhẹ, lazy loading): gộp và nén CSS/JS, kiểm tra lazy loading cho gallery.</t>
+  </si>
+  <si>
+    <t>Kiểm thử toàn bộ hệ thống trên nhiều thiết bị và trình duyệt: Kiểm tra giao diện và chức năng trên nhiều trình duyệt và thiết bị.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xử lý phản hồi của khách hàng (nếu có): Thực hiện các chỉnh sửa cuối cùng dựa trên phản hồi của khách hàng.  </t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Cập nhật báo cáo tiến độ.</t>
+  </si>
+  <si>
+    <t>Hoàn thiện và bàn giao bản demo.</t>
+  </si>
+  <si>
+    <t>Chuẩn bị bản demo hoàn chỉnh: Tạo tệp nén toàn bộ dự án, bao gồm gallery và giao diện trang chủ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viết hướng dẫn sử dụng cho khách hàng: Soạn hướng dẫn quản trị website, cách sử dụng Fancybox, và cập nhật nội dung. </t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email cho khách hàng kèm bản demo và các tài liệu liên quan.</t>
+  </si>
+  <si>
+    <t>Đánh giá và bàn giao chính thức</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Vấn đề: Để bàn giao chính thức vào ngày cuối cùng (hạn chót) có thể gây áp lực nếu phát hiện lỗi sát giờ.</t>
@@ -310,8 +337,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -321,8 +348,8 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>Cải thiện:
@@ -331,147 +358,249 @@
     </r>
   </si>
   <si>
-    <t>Viết mã PHP OOP hoàn thiện gallery và kiểm tra việc hiển thị danh sách hình ảnh trang chủ</t>
-  </si>
-  <si>
-    <t>Chuẩn bị thư mục hình ảnh và chỉnh sửa trang danh sách sản phẩm</t>
-  </si>
-  <si>
-    <t>Chuẩn bị thư mục hình ảnh và chỉnh sửa trang chủ</t>
-  </si>
-  <si>
-    <t>Thiết lập giải pháp lập trình hướng đối tượng cho gallery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xử lý phản hồi của khách hàng (nếu có): Thực hiện các chỉnh sửa cuối cùng dựa trên phản hồi của khách hàng.  </t>
-  </si>
-  <si>
-    <t>Kiểm thử toàn bộ hệ thống trên nhiều thiết bị và trình duyệt: Kiểm tra giao diện và chức năng trên nhiều trình duyệt và thiết bị.</t>
-  </si>
-  <si>
-    <t>Tối ưu hóa mã nguồn(CSS/JS gọn nhẹ, lazy loading): gộp và nén CSS/JS, kiểm tra lazy loading cho gallery.</t>
-  </si>
-  <si>
-    <t>Viết mã PHP OOP hoàn thiện gallery và kiểm tra việc hiển thị danh sách hình ảnh trang danh mục sản phẩm</t>
-  </si>
-  <si>
-    <t>Hiển thị các mục bổ sung trên trang chủ:
-Thêm các hình ảnh như cơ sở pháp lý, bảo hiểm.
-Tích hợp liên kết bảo hiểm vào footer.</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa kích thước hợp lý cho menu, logo, và các thành phần khác theo thiết kế trên màn hình laptop 1366px</t>
-  </si>
-  <si>
-    <t>Gửi báo cáo tiến độ cho khách hàng: Cập nhật trạng thái công việc vào cuối ngày cho khách hàng và đồng đội.</t>
-  </si>
-  <si>
-    <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email yêu cầu khách hàng cung cấp hình ảnh đã duyệt.</t>
-  </si>
-  <si>
-    <t>Gửi báo cáo tiến độ cho khách hàng: Cập nhật báo cáo tiến độ.</t>
-  </si>
-  <si>
-    <t>Gửi báo cáo tiến độ cho khách hàng: Gửi email cho khách hàng kèm bản demo và các tài liệu liên quan.</t>
+    <t>Kiểm tra lần cuối cùng và bàn giao chính thức: Đánh giá toàn bộ hệ thống cùng đồng đội.</t>
+  </si>
+  <si>
+    <t>Sok Kim Thanh
+Lê Duy Anh Tú</t>
+  </si>
+  <si>
+    <t>Xử lý các thay đổi nhỏ nếu có: Kiểm tra lần cuối các chức năng, đảm bảo không có lỗi.</t>
+  </si>
+  <si>
+    <t>Gửi báo cáo tổng kết và bàn giao sản phẩm chính thức cho khách hàng.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,63 +609,234 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -574,162 +874,372 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="16" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="24" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="23" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="23" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="24" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
-        <b val="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+        <family val="2"/>
+        <b val="1"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
         <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF222222"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+        <family val="2"/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
         <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF222222"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+        <family val="2"/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
         <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF222222"/>
+      </font>
+      <numFmt numFmtId="58" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
         <name val="Arial"/>
+        <scheme val="none"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
       </font>
+      <numFmt numFmtId="58" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -737,17 +1247,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -765,7 +1272,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -781,9 +1288,11 @@
               <a:rPr lang="vi-VN"/>
               <a:t>Kế hoạch phát triển website tĩnh CÔNG TY TNHH QUỐC LONG BD </a:t>
             </a:r>
+            <a:endParaRPr lang="vi-VN"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -792,26 +1301,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="vi-VN"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -831,6 +1320,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Kế hoạch chung'!$C$5:$C$17</c:f>
@@ -882,7 +1374,7 @@
             <c:numRef>
               <c:f>'Kế hoạch chung'!$F$5:$F$17</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>45649</c:v>
@@ -926,17 +1418,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-908A-4857-BF33-0624BBCD9B85}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Time</c:v>
+            <c:strRef>
+              <c:f>"Time"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -948,6 +1443,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'Kế hoạch chung'!$G$5:$G$17</c:f>
@@ -996,11 +1494,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-908A-4857-BF33-0624BBCD9B85}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1044,7 +1537,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1056,7 +1549,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="vi-VN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2044195007"/>
@@ -1088,7 +1580,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1104,7 +1596,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1116,7 +1608,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="vi-VN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2044198751"/>
@@ -1133,14 +1624,12 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
+      <c:ext uri="{0b15fc19-7d7d-44ad-8c2d-2c3a37ce22c3}">
+        <chartProps xmlns="https://web.wps.cn/et/2018/main" chartId="{eaa308fe-0f9a-4e3d-8858-58136d061c92}"/>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1162,9 +1651,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="en-US"/>
       </a:pPr>
-      <a:endParaRPr lang="vi-VN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1721,7 +2209,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1735,20 +2223,14 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4428A80C-7018-4477-9E5E-EFD6E7EEBFB3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="617220" y="3676650"/>
+        <a:ext cx="12654915" cy="3638550"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1762,7 +2244,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1771,34 +2253,28 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>5611005</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>1552792</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{237C1CEF-513C-44DD-AE9A-0D9BB00A4C79}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6896100" y="6362700"/>
-          <a:ext cx="5591955" cy="1552792"/>
+          <a:off x="6209030" y="2558415"/>
+          <a:ext cx="5030470" cy="1552575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1822,27 +2298,21 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE492FB4-DE9D-4EE2-8394-A99BC8E69D5B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6900582" y="7574616"/>
-          <a:ext cx="3162741" cy="1838582"/>
+          <a:off x="6209665" y="4199255"/>
+          <a:ext cx="3162935" cy="1838325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1861,32 +2331,26 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3613278</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1220488</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE52A18-9B62-4D4F-A217-DC2B434FC3B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6902264" y="9455523"/>
-          <a:ext cx="3591426" cy="1200318"/>
+          <a:off x="6211570" y="6083300"/>
+          <a:ext cx="3591560" cy="1199515"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1899,15 +2363,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{703F07F9-7C4F-48CD-A7BA-7563727F4EE5}" name="Table1" displayName="Table1" ref="B4:G17" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B4:G17" xr:uid="{703F07F9-7C4F-48CD-A7BA-7563727F4EE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:G17" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B4:G17" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{42F2E47B-6096-43D8-B54E-034E8A83E75A}" name="Giai đoạn" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8CD5CADC-5038-438B-B278-ECD348378C3E}" name="Tên công việc"/>
-    <tableColumn id="3" xr3:uid="{AC4AD0EA-D833-4072-A86E-CCF0D3165D08}" name="Thành viên thực hiện" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{8E9BCE39-129D-4C8E-96E2-1296C1222DB7}" name="Ngày bắt đầu" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{0452BE5B-DB52-44F6-89DC-E21AE61F6C8C}" name="Ngày kết thúc" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{37D6A49B-E662-4F07-8FC3-55DDBFF9C668}" name="Số giờ làm việc một ngày"/>
+    <tableColumn id="1" name="Giai đoạn" dataDxfId="0"/>
+    <tableColumn id="2" name="Tên công việc"/>
+    <tableColumn id="3" name="Thành viên thực hiện" dataDxfId="1"/>
+    <tableColumn id="4" name="Ngày bắt đầu" dataDxfId="2"/>
+    <tableColumn id="5" name="Ngày kết thúc" dataDxfId="3"/>
+    <tableColumn id="7" name="Số giờ làm việc một ngày"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1956,7 +2420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1991,7 +2455,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2165,314 +2629,309 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="26.125" customWidth="1"/>
-    <col min="3" max="3" width="53.875" customWidth="1"/>
-    <col min="4" max="7" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="26.1296296296296" customWidth="1"/>
+    <col min="3" max="3" width="53.8796296296296" customWidth="1"/>
+    <col min="4" max="7" width="26.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="1" spans="2:7">
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5">
         <v>45645</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>45649</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="2:7">
+      <c r="B6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5">
         <v>45645</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>45648</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="2:7">
+      <c r="B7" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
         <v>45648</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="5">
         <v>45649</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>2</v>
+    <row r="8" spans="2:7">
+      <c r="B8" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="E8" s="28">
         <v>45649</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="28">
         <v>45651</v>
       </c>
       <c r="G8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="5">
+    <row r="9" spans="2:7">
+      <c r="B9" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="28">
         <v>45650</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="28">
         <v>45653</v>
       </c>
       <c r="G9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
+    <row r="10" spans="2:7">
+      <c r="B10" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="5">
+      <c r="C10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="28">
         <v>45653</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="28">
         <v>45656</v>
       </c>
       <c r="G10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>5</v>
+    <row r="11" spans="2:7">
+      <c r="B11" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="5">
+        <v>18</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="28">
         <v>45653</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="28">
         <v>45656</v>
       </c>
       <c r="G11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>5</v>
+    <row r="12" spans="2:7">
+      <c r="B12" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5">
+        <v>18</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="28">
         <v>45653</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="28">
         <v>45656</v>
       </c>
       <c r="G12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
+    <row r="13" spans="2:7">
+      <c r="B13" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="5">
+        <v>19</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="28">
         <v>45657</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="28">
         <v>45658</v>
       </c>
       <c r="G13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>5</v>
+    <row r="14" spans="2:7">
+      <c r="B14" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="5">
+        <v>20</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="28">
         <v>45657</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="28">
         <v>45658</v>
       </c>
       <c r="G14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>8</v>
+    <row r="15" spans="2:7">
+      <c r="B15" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="5">
+        <v>22</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="28">
         <v>45659</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="28">
         <v>45660</v>
       </c>
       <c r="G15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>8</v>
+    <row r="16" spans="2:7">
+      <c r="B16" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D16" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="28">
         <v>45659</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="28">
         <v>45661</v>
       </c>
       <c r="G16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>8</v>
+    <row r="17" spans="2:7">
+      <c r="B17" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="D17" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="28">
         <v>45659</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="28">
         <v>45661</v>
       </c>
       <c r="G17">
@@ -2484,680 +2943,692 @@
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC3744B-6692-456B-A13C-CDD2B8AE7919}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr filterMode="1"/>
   <dimension ref="C5:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="4" width="36.125" customWidth="1"/>
-    <col min="5" max="5" width="73.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="36.1296296296296" customWidth="1"/>
+    <col min="5" max="5" width="73.6296296296296" customWidth="1"/>
+    <col min="6" max="6" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.6296296296296" customWidth="1"/>
+    <col min="10" max="10" width="15.6296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="3:10">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1" spans="3:10">
       <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="13"/>
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4"/>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5">
         <v>45651</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="5">
         <v>45652</v>
       </c>
       <c r="J6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="10"/>
-      <c r="E7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="8"/>
+    <row r="7" spans="4:10">
+      <c r="D7" s="2"/>
+      <c r="E7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="7"/>
       <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="3">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5">
         <v>45651</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="5">
         <v>45652</v>
       </c>
       <c r="J7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D8" s="10"/>
-      <c r="E8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="13"/>
+    <row r="8" hidden="1" spans="4:10">
+      <c r="D8" s="2"/>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3">
+        <v>9</v>
+      </c>
+      <c r="H8" s="5">
         <v>45651</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="5">
         <v>45652</v>
       </c>
       <c r="J8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D9" s="10"/>
-      <c r="E9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="8"/>
+    <row r="9" ht="28.8" spans="4:10">
+      <c r="D9" s="2"/>
+      <c r="E9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7"/>
       <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="3">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5">
         <v>45651</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="5">
         <v>45652</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D10" s="10"/>
-      <c r="E10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="22"/>
+    <row r="10" hidden="1" spans="4:10">
+      <c r="D10" s="2"/>
+      <c r="E10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8"/>
       <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="3">
+        <v>9</v>
+      </c>
+      <c r="H10" s="5">
         <v>45651</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="5">
         <v>45652</v>
       </c>
       <c r="J10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D11" s="10"/>
-      <c r="E11" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="20"/>
+    <row r="11" ht="28.8" hidden="1" spans="4:10">
+      <c r="D11" s="2"/>
+      <c r="E11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="10"/>
       <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="3">
+        <v>9</v>
+      </c>
+      <c r="H11" s="5">
         <v>45651</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="5">
         <v>45652</v>
       </c>
       <c r="J11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="10"/>
-      <c r="E12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="13"/>
+    <row r="12" hidden="1" spans="4:10">
+      <c r="D12" s="2"/>
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="4"/>
       <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="3">
+        <v>9</v>
+      </c>
+      <c r="H12" s="5">
         <v>45651</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="5">
         <v>45652</v>
       </c>
       <c r="J12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D13" s="10"/>
-      <c r="E13" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="8"/>
+    <row r="13" hidden="1" spans="4:10">
+      <c r="D13" s="2"/>
+      <c r="E13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="3">
+        <v>9</v>
+      </c>
+      <c r="H13" s="5">
         <v>45651</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="5">
         <v>45652</v>
       </c>
       <c r="J13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D14" s="10"/>
-      <c r="E14" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="8"/>
+    <row r="14" spans="4:10">
+      <c r="D14" s="2"/>
+      <c r="E14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="7"/>
       <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="3">
+        <v>11</v>
+      </c>
+      <c r="H14" s="5">
         <v>45651</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="5">
         <v>45652</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" ht="28.5" hidden="1" customHeight="1" spans="3:10">
       <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="23"/>
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="12"/>
       <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="3">
+        <v>9</v>
+      </c>
+      <c r="H15" s="5">
         <v>45652</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="5">
         <v>45653</v>
       </c>
       <c r="J15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D16" s="10"/>
-      <c r="E16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="8"/>
+    <row r="16" ht="28.8" hidden="1" spans="4:10">
+      <c r="D16" s="2"/>
+      <c r="E16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="7"/>
       <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="3">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5">
         <v>45652</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="5">
         <v>45653</v>
       </c>
       <c r="J16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D17" s="10"/>
-      <c r="E17" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="8"/>
+    <row r="17" ht="28.8" hidden="1" spans="4:10">
+      <c r="D17" s="2"/>
+      <c r="E17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="7"/>
       <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="3">
+        <v>9</v>
+      </c>
+      <c r="H17" s="5">
         <v>45652</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="5">
         <v>45653</v>
       </c>
       <c r="J17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D18" s="10"/>
-      <c r="E18" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="19"/>
+    <row r="18" ht="28.8" hidden="1" spans="4:10">
+      <c r="D18" s="2"/>
+      <c r="E18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="13"/>
       <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="3">
+        <v>9</v>
+      </c>
+      <c r="H18" s="5">
         <v>45652</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="5">
         <v>45653</v>
       </c>
       <c r="J18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="19" ht="43.2" hidden="1" spans="3:10">
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="8"/>
+        <v>48</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="7"/>
       <c r="G19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="3">
+        <v>9</v>
+      </c>
+      <c r="H19" s="5">
         <v>45653</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="5">
         <v>45654</v>
       </c>
       <c r="J19">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D20" s="10"/>
-      <c r="E20" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="8"/>
+    <row r="20" ht="28.8" hidden="1" spans="4:10">
+      <c r="D20" s="2"/>
+      <c r="E20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="3">
+        <v>9</v>
+      </c>
+      <c r="H20" s="5">
         <v>45653</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="5">
         <v>45654</v>
       </c>
       <c r="J20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D21" s="10"/>
-      <c r="E21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="24"/>
+    <row r="21" ht="28.8" spans="4:10">
+      <c r="D21" s="2"/>
+      <c r="E21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="14"/>
       <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="3">
+        <v>11</v>
+      </c>
+      <c r="H21" s="5">
         <v>45653</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="5">
         <v>45654</v>
       </c>
       <c r="J21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D22" s="10"/>
-      <c r="E22" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="8"/>
+    <row r="22" ht="28.8" spans="4:10">
+      <c r="D22" s="2"/>
+      <c r="E22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="3">
+        <v>11</v>
+      </c>
+      <c r="H22" s="5">
         <v>45653</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="5">
         <v>45654</v>
       </c>
       <c r="J22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="3:10" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="10"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="8"/>
+    <row r="23" ht="127.5" customHeight="1" spans="4:10">
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
       <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="3">
+        <v>11</v>
+      </c>
+      <c r="H23" s="5">
         <v>45653</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="5">
         <v>45654</v>
       </c>
       <c r="J23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="3:10" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="10"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="8"/>
+    <row r="24" ht="148.5" customHeight="1" spans="4:10">
+      <c r="D24" s="2"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
       <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="3">
+        <v>11</v>
+      </c>
+      <c r="H24" s="5">
         <v>45653</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="5">
         <v>45654</v>
       </c>
       <c r="J24">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="3:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="10"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="8"/>
+    <row r="25" ht="96" customHeight="1" spans="4:10">
+      <c r="D25" s="2"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
       <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="3">
+        <v>11</v>
+      </c>
+      <c r="H25" s="5">
         <v>45653</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="5">
         <v>45654</v>
       </c>
       <c r="J25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D26" s="10"/>
-      <c r="E26" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="20"/>
+    <row r="26" ht="28.8" hidden="1" spans="4:10">
+      <c r="D26" s="2"/>
+      <c r="E26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="10"/>
       <c r="G26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="3">
+        <v>9</v>
+      </c>
+      <c r="H26" s="5">
         <v>45653</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="5">
         <v>45654</v>
       </c>
       <c r="J26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" ht="28.5" customHeight="1" spans="3:10">
       <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>61</v>
+      <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="3">
+        <v>11</v>
+      </c>
+      <c r="H27" s="5">
         <v>45654</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="5">
         <v>45655</v>
       </c>
       <c r="J27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D28" s="10"/>
-      <c r="E28" s="12" t="s">
-        <v>60</v>
+    <row r="28" ht="28.8" spans="4:10">
+      <c r="D28" s="2"/>
+      <c r="E28" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="3">
+        <v>11</v>
+      </c>
+      <c r="H28" s="5">
         <v>45654</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="5">
         <v>45655</v>
       </c>
       <c r="J28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D29" s="10"/>
-      <c r="E29" s="12" t="s">
-        <v>59</v>
+    <row r="29" ht="28.8" spans="4:10">
+      <c r="D29" s="2"/>
+      <c r="E29" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="3">
+        <v>11</v>
+      </c>
+      <c r="H29" s="5">
         <v>45654</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="5">
         <v>45655</v>
       </c>
       <c r="J29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D30" s="10"/>
-      <c r="E30" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="14"/>
+    <row r="30" spans="4:10">
+      <c r="D30" s="2"/>
+      <c r="E30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="17"/>
       <c r="G30" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="3">
+        <v>11</v>
+      </c>
+      <c r="H30" s="5">
         <v>45654</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="5">
         <v>45655</v>
       </c>
       <c r="J30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" ht="28.8" hidden="1" spans="3:10">
       <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="12" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="3">
+        <v>9</v>
+      </c>
+      <c r="H31" s="5">
         <v>45655</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="5">
         <v>45656</v>
       </c>
       <c r="J31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D32" s="10"/>
-      <c r="E32" s="12" t="s">
-        <v>46</v>
+    <row r="32" ht="28.8" hidden="1" spans="4:10">
+      <c r="D32" s="2"/>
+      <c r="E32" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="F32" s="16"/>
       <c r="G32" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="3">
+        <v>9</v>
+      </c>
+      <c r="H32" s="5">
         <v>45655</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="5">
         <v>45656</v>
       </c>
       <c r="J32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D33" s="10"/>
-      <c r="E33" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="21"/>
+    <row r="33" ht="28.8" hidden="1" spans="4:10">
+      <c r="D33" s="2"/>
+      <c r="E33" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="18"/>
       <c r="G33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="3">
+        <v>9</v>
+      </c>
+      <c r="H33" s="5">
         <v>45655</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="5">
         <v>45656</v>
       </c>
       <c r="J33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" ht="28.5" customHeight="1" spans="3:10">
       <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="3">
+        <v>63</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34" s="5">
         <v>45656</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="5">
         <v>45657</v>
       </c>
       <c r="J34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="D35" s="10"/>
-      <c r="E35" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="3">
+    <row r="35" ht="28.8" spans="4:10">
+      <c r="D35" s="2"/>
+      <c r="E35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="5">
         <v>45656</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="5">
         <v>45657</v>
       </c>
       <c r="J35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D36" s="10"/>
-      <c r="E36" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="27"/>
+    <row r="36" ht="85.5" hidden="1" customHeight="1" spans="4:10">
+      <c r="D36" s="2"/>
+      <c r="E36" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="3">
+        <v>9</v>
+      </c>
+      <c r="H36" s="5">
         <v>45656</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="5">
         <v>45657</v>
       </c>
       <c r="J36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="D37" s="11"/>
+    <row r="37" spans="4:4">
+      <c r="D37" s="24"/>
     </row>
   </sheetData>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="C5:J36" etc:filterBottomFollowUsedRange="0">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Sok Kim Thanh&#10;Lê Duy Anh Tú"/>
+        <filter val="Lê Duy Anh Tú"/>
+      </filters>
+    </filterColumn>
+    <extLst/>
+  </autoFilter>
   <mergeCells count="4">
-    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D6:D14"/>
     <mergeCell ref="D15:D26"/>
     <mergeCell ref="D27:D33"/>
-    <mergeCell ref="D6:D14"/>
+    <mergeCell ref="D34:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>